<commit_message>
Advances on consolidated report, needs to test out
</commit_message>
<xml_diff>
--- a/data/Consolidated_Template.xlsx
+++ b/data/Consolidated_Template.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unhcr365-my.sharepoint.com/personal/fayolle_unhcr_org/Documents/Documents/GitHub/RMRP2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="782" documentId="8_{7895EE31-5926-4FE0-8CE3-983282D3319B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E29020C-3EEE-49B3-AA4B-3EC7D4F59336}"/>
+  <xr:revisionPtr revIDLastSave="787" documentId="8_{7895EE31-5926-4FE0-8CE3-983282D3319B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A2DA23E-80AD-47B9-B575-F04631665AB5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="843" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="28845" yWindow="1530" windowWidth="21600" windowHeight="11325" tabRatio="843" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Countries" sheetId="27" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Countries'!$A$1:$E$2969</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1193,7 +1196,7 @@
   <dimension ref="A1:E2969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B226" sqref="B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51678,6 +51681,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E2969" xr:uid="{0BCCFB69-8466-461D-94F0-09FAA61D5A73}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>